<commit_message>
can't get it to param estimate log transformed x input
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,12 +487,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3.76</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed fake low input data
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weiss Lab\Documents\Jupyter Notebooks\Curve-Fitting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas DeLateur\JupyterNotebooks\Curve Fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,39 +456,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1">
-        <v>4.0999999999999996</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="B16">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Now for hill functions
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas DeLateur\JupyterNotebooks\Curve Fitting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\Jupyter Notebooks\Curve-Fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="6525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>lasAHL_nM</t>
+    <t>x</t>
   </si>
   <si>
-    <t>MEFL_geomean</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,11 +349,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Making the pandas more smart
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\Jupyter Notebooks\Curve-Fitting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weiss Lab\Documents\Jupyter Notebooks\Curve-Fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="6525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>x</t>
+    <t>GFP (geometric mean MEFL)</t>
   </si>
   <si>
-    <t>y</t>
+    <t>lasAHL (nM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,21 +349,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fits log log to better parameter estimate basal expression
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="B13" s="1">
         <v>3.76</v>

</xml_diff>

<commit_message>
Actually using pLas data from pL2f1417
</commit_message>
<xml_diff>
--- a/HillTestData.xlsx
+++ b/HillTestData.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,7 +375,7 @@
         <v>2000</v>
       </c>
       <c r="B2" s="1">
-        <v>648</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -383,7 +383,7 @@
         <v>1000</v>
       </c>
       <c r="B3" s="1">
-        <v>652</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>500</v>
       </c>
       <c r="B4" s="1">
-        <v>629</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -399,7 +399,7 @@
         <v>100</v>
       </c>
       <c r="B5" s="1">
-        <v>568</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -407,7 +407,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="1">
-        <v>571</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -415,7 +415,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>203</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -423,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>179</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,7 +431,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>71.2</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
         <v>0.5</v>
       </c>
       <c r="B10" s="1">
-        <v>39.299999999999997</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>0.1</v>
       </c>
       <c r="B11" s="1">
-        <v>5.28</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +455,7 @@
         <v>0.05</v>
       </c>
       <c r="B12" s="1">
-        <v>4.7300000000000004</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,16 +463,12 @@
         <v>0.01</v>
       </c>
       <c r="B13" s="1">
-        <v>3.76</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>3.76</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>